<commit_message>
comment added to the jobspage, some methods renamed
</commit_message>
<xml_diff>
--- a/target/test-classes/data.xlsx
+++ b/target/test-classes/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirek\IdeaProjects\GetDataFromWorkPortals\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F41BC4-F1FF-480F-A44C-F985FF0AB719}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED07D75-831F-4FC7-8A2D-73256E1EF1D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4C8D30A-BB96-4518-832A-65DDBDCBD732}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD33"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
detailInfoElement added, getDetailedInformation method edited
</commit_message>
<xml_diff>
--- a/target/test-classes/data.xlsx
+++ b/target/test-classes/data.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mirek\IdeaProjects\GetDataFromWorkPortals\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED07D75-831F-4FC7-8A2D-73256E1EF1D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9216272A-965F-4A14-994F-8487B0DAEDAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4C8D30A-BB96-4518-832A-65DDBDCBD732}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="96">
   <si>
     <t>TIMESTAMP</t>
   </si>
@@ -58,12 +58,277 @@
   </si>
   <si>
     <t>DETAIL</t>
+  </si>
+  <si>
+    <t>06.04.2021 10:38</t>
+  </si>
+  <si>
+    <t>jobs.cz</t>
+  </si>
+  <si>
+    <t>Design System Architekt pro Seduo.cz</t>
+  </si>
+  <si>
+    <t>LMC s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1555558490/</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Práce převážně z domova</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>PHP/React Developer/ka v týmu Jobs.cz</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1544481482/</t>
+  </si>
+  <si>
+    <t>Možnost občasné práce z domova</t>
+  </si>
+  <si>
+    <t>PHP/JS Developer(ka) pro Atmoskop.cz - projekt do konce roku</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1554774674/</t>
+  </si>
+  <si>
+    <t>ITSM Consultant</t>
+  </si>
+  <si>
+    <t>Eller, s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1556336089/</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>SAP Business Analyst</t>
+  </si>
+  <si>
+    <t>DRILL Business Services</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1557673551/</t>
+  </si>
+  <si>
+    <t>L1 Global Security Operations Center (GSOC) Analyst 24/7</t>
+  </si>
+  <si>
+    <t>Devoteam, s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1556173164/</t>
+  </si>
+  <si>
+    <t>Problem Manager</t>
+  </si>
+  <si>
+    <t>MONETA Money</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1556799562/</t>
+  </si>
+  <si>
+    <t>06.04.2021 10:39</t>
+  </si>
+  <si>
+    <t>Scrum master</t>
+  </si>
+  <si>
+    <t>Skupina Amper</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1556161443/</t>
+  </si>
+  <si>
+    <t>Junior konzultant – systémový specialista podpory ESS</t>
+  </si>
+  <si>
+    <t>GORDIC spol. s r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1548641737/</t>
+  </si>
+  <si>
+    <t>Team Lead- Biometric Solutions</t>
+  </si>
+  <si>
+    <t>Thales DIS Czech Republic s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1551192620/</t>
+  </si>
+  <si>
+    <t>Data Scientist for Time Series Forecasting</t>
+  </si>
+  <si>
+    <t>Deutsche Telekom Services Europe Czech Republic s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1557671288/</t>
+  </si>
+  <si>
+    <t>TRADER / MATEMATICKÝ ANALYTIK | ALGORITMICKÝ TRADING</t>
+  </si>
+  <si>
+    <t>Talentica s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1557667649/</t>
+  </si>
+  <si>
+    <t>40 000 – 80 000 Kč</t>
+  </si>
+  <si>
+    <t>IT Projektový manažer - projektová metodika (m/ž)</t>
+  </si>
+  <si>
+    <t>HCL TECHNOLOGIES CZECH REPUBLIC s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1556690923/</t>
+  </si>
+  <si>
+    <t>IT Projektový manažer - Quality Assurance (m/ž)</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1556692490/</t>
+  </si>
+  <si>
+    <t>Junior konzultant Helios Orange</t>
+  </si>
+  <si>
+    <t>TPA</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1536467801/</t>
+  </si>
+  <si>
+    <t>IT Analytik - Integrace / Cards &amp; Payments</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1553016765/</t>
+  </si>
+  <si>
+    <t>Systémový inženýr – Voice specialista</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1555286171/</t>
+  </si>
+  <si>
+    <t>TESTER - Developer automatizovaných testů pro web</t>
+  </si>
+  <si>
+    <t>Rockwell Automation s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1489006918/</t>
+  </si>
+  <si>
+    <t>Test Automation Consultant</t>
+  </si>
+  <si>
+    <t>cz.MicroNova s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1553760382/</t>
+  </si>
+  <si>
+    <t>Konzultant pro oblast integrací</t>
+  </si>
+  <si>
+    <t>AIMTEC a.s.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1556618481/</t>
+  </si>
+  <si>
+    <t>Group Android Developer</t>
+  </si>
+  <si>
+    <t>FORTUNA GAME a.s.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1555844567/</t>
+  </si>
+  <si>
+    <t>Group Front End Developer - Vue.js</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1555843901/</t>
+  </si>
+  <si>
+    <t>Group Python Developer</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1555843498/</t>
+  </si>
+  <si>
+    <t>Group Senior Configuration Specialist</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1552097376/</t>
+  </si>
+  <si>
+    <t>Group Configuration Specialist</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1534205316/</t>
+  </si>
+  <si>
+    <t>Cloud Security Analyst</t>
+  </si>
+  <si>
+    <t>Kooperativa pojišťovna, a.s., VIG</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1549489511/</t>
+  </si>
+  <si>
+    <t>Senior JAVA Developer - Middle Office Platform</t>
+  </si>
+  <si>
+    <t>Capgemini Czech Republic s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1550808498/</t>
+  </si>
+  <si>
+    <t>Senior JAVA Developer - Central Risk</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1550366199/</t>
+  </si>
+  <si>
+    <t>Senior .NET Developer - Delta-1 Front Office team</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1550812796/</t>
+  </si>
+  <si>
+    <t>Service Delivery Manager</t>
+  </si>
+  <si>
+    <t>NEECO s.r.o.</t>
+  </si>
+  <si>
+    <t>https://www.jobs.cz/rpd/1557666550/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,21 +675,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9B2CFC-478A-4BBD-9936-02EEE9F01803}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A2" sqref="A2:XFD151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="63" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="41.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="44.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="63.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="44.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -453,6 +718,786 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>